<commit_message>
add burn area effect
</commit_message>
<xml_diff>
--- a/network/case1/case1_fire_route.xlsx
+++ b/network/case1/case1_fire_route.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\專題研究\code\githubrepo\final\network\case1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5062EA3-33C3-4495-BC18-134BEA14AC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25F526E-BA05-44C8-9125-E617F347D965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -403,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -433,24 +446,28 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>207.6342938919291</v>
+        <f ca="1">RANDBETWEEN(20,40)</f>
+        <v>22</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <f ca="1">RANDBETWEEN(10,15)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>207.6342938919291</v>
+        <f t="shared" ref="C3:C66" ca="1" si="0">RANDBETWEEN(20,40)</f>
+        <v>31</v>
       </c>
       <c r="D3">
-        <v>18</v>
+        <f t="shared" ref="D3:D66" ca="1" si="1">RANDBETWEEN(10,15)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -458,293 +475,335 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
       </c>
       <c r="D5">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="D7">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
       </c>
       <c r="D8">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
       </c>
       <c r="D9">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
       </c>
       <c r="D10">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
         <v>6</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
       <c r="C11">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="D12">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
       </c>
       <c r="D13">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="D15">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
         <v>3</v>
       </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
       <c r="C16">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="D16">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
       </c>
       <c r="D17">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="D18">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="D19">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="D20">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="D21">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="D22">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
       </c>
       <c r="D23">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C24">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
       </c>
       <c r="D24">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -755,24 +814,28 @@
         <v>7</v>
       </c>
       <c r="C25">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="D25">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B26">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
       </c>
       <c r="D26">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -780,27 +843,31 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
       </c>
       <c r="D27">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="D28">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -808,27 +875,31 @@
         <v>9</v>
       </c>
       <c r="B29">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C29">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="D29">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
       </c>
       <c r="D30">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -836,27 +907,31 @@
         <v>10</v>
       </c>
       <c r="B31">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
       </c>
       <c r="D31">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
         <v>9</v>
       </c>
-      <c r="B32">
-        <v>10</v>
-      </c>
       <c r="C32">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
       </c>
       <c r="D32">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -864,69 +939,79 @@
         <v>10</v>
       </c>
       <c r="B33">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C33">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
       </c>
       <c r="D33">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C34">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="D34">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C35">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="D35">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C36">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C37">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
       </c>
       <c r="D37">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -934,27 +1019,31 @@
         <v>11</v>
       </c>
       <c r="B38">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C38">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
       </c>
       <c r="D38">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C39">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="D39">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -962,27 +1051,31 @@
         <v>12</v>
       </c>
       <c r="B40">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
       </c>
       <c r="D40">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B41">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C41">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
       </c>
       <c r="D41">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -990,55 +1083,63 @@
         <v>13</v>
       </c>
       <c r="B42">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C42">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
       </c>
       <c r="D42">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B43">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C43">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
       </c>
       <c r="D43">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B44">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C44">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
       </c>
       <c r="D44">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
       </c>
       <c r="D45">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1046,83 +1147,95 @@
         <v>14</v>
       </c>
       <c r="B46">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C46">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
       </c>
       <c r="D46">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B47">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C47">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
       </c>
       <c r="D47">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B48">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="D48">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B49">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
       </c>
       <c r="D49">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
       </c>
       <c r="D50">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B51">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C51">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="D51">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1130,55 +1243,63 @@
         <v>16</v>
       </c>
       <c r="B52">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C52">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
       </c>
       <c r="D52">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B53">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C53">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
       </c>
       <c r="D53">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C54">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
       </c>
       <c r="D54">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B55">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C55">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
       </c>
       <c r="D55">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1186,27 +1307,31 @@
         <v>17</v>
       </c>
       <c r="B56">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C56">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
       </c>
       <c r="D56">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B57">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C57">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
       </c>
       <c r="D57">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1214,27 +1339,31 @@
         <v>17</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C58">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
       </c>
       <c r="D58">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
+        <v>17</v>
+      </c>
+      <c r="B59">
         <v>20</v>
       </c>
-      <c r="B59">
-        <v>17</v>
-      </c>
       <c r="C59">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>40</v>
       </c>
       <c r="D59">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1242,83 +1371,95 @@
         <v>18</v>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C60">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
       </c>
       <c r="D60">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B61">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C61">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>39</v>
       </c>
       <c r="D61">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B62">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C62">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
       </c>
       <c r="D62">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
+        <v>19</v>
+      </c>
+      <c r="B63">
+        <v>16</v>
+      </c>
+      <c r="C63">
+        <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
-      <c r="B63">
-        <v>20</v>
-      </c>
-      <c r="C63">
-        <v>207.6342938919291</v>
-      </c>
       <c r="D63">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B64">
+        <v>17</v>
+      </c>
+      <c r="C64">
+        <f t="shared" ca="1" si="0"/>
         <v>22</v>
       </c>
-      <c r="C64">
-        <v>207.6342938919291</v>
-      </c>
       <c r="D64">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B65">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C65">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
       </c>
       <c r="D65">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1326,27 +1467,31 @@
         <v>20</v>
       </c>
       <c r="B66">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C66">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
       </c>
       <c r="D66">
-        <v>18</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B67">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C67">
-        <v>207.6342938919291</v>
+        <f t="shared" ref="C67:C77" ca="1" si="2">RANDBETWEEN(20,40)</f>
+        <v>35</v>
       </c>
       <c r="D67">
-        <v>18</v>
+        <f t="shared" ref="D67:D77" ca="1" si="3">RANDBETWEEN(10,15)</f>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1354,251 +1499,159 @@
         <v>21</v>
       </c>
       <c r="B68">
+        <v>13</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ca="1" si="2"/>
         <v>23</v>
       </c>
-      <c r="C68">
-        <v>207.6342938919291</v>
-      </c>
       <c r="D68">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B69">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C69">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
       </c>
       <c r="D69">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B70">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C70">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>36</v>
       </c>
       <c r="D70">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B71">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C71">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
       </c>
       <c r="D71">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B72">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C72">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>31</v>
       </c>
       <c r="D72">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B73">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C73">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
       </c>
       <c r="D73">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B74">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C74">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>38</v>
       </c>
       <c r="D74">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C75">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>32</v>
       </c>
       <c r="D75">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C76">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>33</v>
       </c>
       <c r="D76">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B77">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C77">
-        <v>207.6342938919291</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
       </c>
       <c r="D77">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>13</v>
-      </c>
-      <c r="B78">
-        <v>19</v>
-      </c>
-      <c r="C78">
-        <v>207.6342938919291</v>
-      </c>
-      <c r="D78">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>19</v>
-      </c>
-      <c r="B79">
-        <v>13</v>
-      </c>
-      <c r="C79">
-        <v>207.6342938919291</v>
-      </c>
-      <c r="D79">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>13</v>
-      </c>
-      <c r="B80">
-        <v>15</v>
-      </c>
-      <c r="C80">
-        <v>207.6342938919291</v>
-      </c>
-      <c r="D80">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>15</v>
-      </c>
-      <c r="B81">
-        <v>13</v>
-      </c>
-      <c r="C81">
-        <v>207.6342938919291</v>
-      </c>
-      <c r="D81">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82">
-        <v>19</v>
-      </c>
-      <c r="B82">
-        <v>20</v>
-      </c>
-      <c r="C82">
-        <v>207.6342938919291</v>
-      </c>
-      <c r="D82">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83">
-        <v>20</v>
-      </c>
-      <c r="B83">
-        <v>19</v>
-      </c>
-      <c r="C83">
-        <v>207.6342938919291</v>
-      </c>
-      <c r="D83">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84">
-        <v>19</v>
-      </c>
-      <c r="B84">
-        <v>21</v>
-      </c>
-      <c r="C84">
-        <v>207.6342938919291</v>
-      </c>
-      <c r="D84">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>21</v>
-      </c>
-      <c r="B85">
-        <v>19</v>
-      </c>
-      <c r="C85">
-        <v>207.6342938919291</v>
-      </c>
-      <c r="D85">
-        <v>18</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>